<commit_message>
change in import file formats
</commit_message>
<xml_diff>
--- a/SageFrame/Modules/AspxCommerce/AspxImportManager/Uploads/eCommerce Data Entry online.xlsx
+++ b/SageFrame/Modules/AspxCommerce/AspxImportManager/Uploads/eCommerce Data Entry online.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
-  <si>
-    <t>Category</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+  <si>
+    <t>Category Name:</t>
   </si>
   <si>
     <t>SKU Code:</t>
@@ -51,6 +51,9 @@
     <t>Seller Information:</t>
   </si>
   <si>
+    <t>Currency Code:</t>
+  </si>
+  <si>
     <t>Price:</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
     <t>estestt etgdsg</t>
   </si>
   <si>
+    <t>USD</t>
+  </si>
+  <si>
     <t>ecommerce, online shopping, nepal</t>
   </si>
   <si>
@@ -132,16 +138,79 @@
     <t>Used</t>
   </si>
   <si>
-    <t>CAt1/Sub-cat2/Sub-cat3</t>
+    <t>sfdsf</t>
+  </si>
+  <si>
+    <t>dsfdsf</t>
   </si>
   <si>
     <t>fdsf</t>
   </si>
   <si>
-    <t>fsdaf</t>
-  </si>
-  <si>
     <t>fdsaf</t>
+  </si>
+  <si>
+    <t>dasfd</t>
+  </si>
+  <si>
+    <t>fdsfa.jpg</t>
+  </si>
+  <si>
+    <t>fdsafd.jpg</t>
+  </si>
+  <si>
+    <t>Not Specified</t>
+  </si>
+  <si>
+    <t>fdsafdsafdsaf</t>
+  </si>
+  <si>
+    <t>ecommerce, online shopping, nepalsss</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>!WEIGHT</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>!CostVariantOption</t>
+  </si>
+  <si>
+    <t>!CostVariantValue</t>
+  </si>
+  <si>
+    <t>!DISPLAY_ORDER</t>
+  </si>
+  <si>
+    <t>!IMAGE</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>a.jpg,b.jpg</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>30ml</t>
+  </si>
+  <si>
+    <t>60ml</t>
   </si>
 </sst>
 </file>
@@ -157,12 +226,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -188,11 +263,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -217,11 +296,11 @@
 
 <file path=xl/surveys/survey1.xml><?xml version="1.0" encoding="utf-8"?>
 <survey xmlns="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" id="1" guid="{64B1BA67-1E85-4E60-A646-329F4E5B105B}" title="eCommerce Data Entry" description="You need to go to the local market and fill this form from each sellers and dealers">
-  <surveyPr cssClass="acc-form-designer acc-surveyform" width="492" height="2671" position="relative"/>
+  <surveyPr cssClass="acc-form-designer acc-surveyform" width="492" height="2767" position="relative"/>
   <titlePr cssClass="acc-surveyform-title" top="30" left="30" width="432" height="55" position="absolute"/>
   <descriptionPr cssClass="acc-surveyform-description" top="90" left="30" width="432" height="67" position="absolute"/>
   <questions>
-    <questionsPr top="162" left="30" width="432" height="2479" position="absolute"/>
+    <questionsPr top="162" left="30" width="432" height="2575" position="absolute"/>
     <question binding="1" text="Category Name:" type="singleLineOfText" helpText="e.g. &lt;Parent Category Name&gt;/&lt;Child Category Name&gt;/&lt;Sub-Category Name&gt;" defaultValue="CAt1/Sub-cat2/Sub-cat3">
       <questionPr top="1" left="1" width="432" height="79" position="absolute"/>
     </question>
@@ -255,60 +334,63 @@
     <question binding="11" text="Seller Information:" type="multipleLinesOfText" helpText="Write detail about the seller- contact address, number and map" required="1">
       <questionPr top="981" left="1" width="432" height="149" position="absolute"/>
     </question>
+    <question binding="29" text="Currency Code:" type="singleLineOfText" helpText="Write in which currency code this price is:_x000a_e.g. : USD, NPR" required="1" defaultValue="USD">
+      <questionPr top="1135" left="1" width="432" height="93" position="absolute"/>
+    </question>
     <question binding="12" text="Price:" type="number" format="fixed" helpText="What is the regular price of the item?" defaultValue="1.00">
-      <questionPr top="1135" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1233" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="13" text="Cost Price:" type="number" format="fixed" helpText="What is the cost price of the item?" required="1" defaultValue="1.00">
-      <questionPr top="1219" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1317" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="14" text="List Price:" type="number" format="fixed" helpText="What is the price you will be selling?" defaultValue="1.00">
-      <questionPr top="1303" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1401" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="15" text="Manufacturer Suggested Retail Price (MRP):" type="number" format="fixed" helpText="What is the MRP for this item?" defaultValue="1.00">
-      <questionPr top="1387" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1485" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="16" text="Meta Description:" type="multipleLinesOfText" helpText="For SEO write the meta description" defaultValue="ecommerce, online shopping, nepal">
-      <questionPr top="1471" left="1" width="432" height="149" position="absolute"/>
+      <questionPr top="1569" left="1" width="432" height="149" position="absolute"/>
     </question>
     <question binding="17" text="Meta Keyword:" type="singleLineOfText" helpText="For SEO write the meta keywords" defaultValue="ecommerce, online shopping, nepal">
-      <questionPr top="1625" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1723" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="18" text="Meta Title:" type="singleLineOfText" helpText="For SEO write the meta Title" defaultValue="ecommerce, online shopping, nepal">
-      <questionPr top="1709" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1807" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="19" text="Length:" type="number" format="fixed" helpText="What is the length of the item?" required="1" defaultValue="0.00">
-      <questionPr top="1793" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1891" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="20" text="Height:" type="number" format="fixed" helpText="What is the height of the item?" required="1" defaultValue="0.00">
-      <questionPr top="1877" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="1975" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="21" text="Width:" type="number" format="fixed" helpText="What is the width of the item?" required="1" defaultValue="0.00">
-      <questionPr top="1961" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="2059" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="22" text="Is Featured:" type="choice" helpText="Do you want to make this item featured on our site and showcase on front?" required="1" defaultValue="FALSE" rowSource="TRUE;FALSE">
-      <questionPr top="2045" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="2143" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="23" text="Is Special:" type="choice" helpText="Do you want to showcase this item as special?" required="1" defaultValue="FALSE" rowSource="TRUE;FALSE">
-      <questionPr top="2129" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="2227" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="24" text="Special Price:" type="number" format="fixed" helpText="Specify if seller want to low the price for some special occasions and date range">
-      <questionPr top="2213" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="2311" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="25" text="Special Price From Date:" type="date" helpText="Only specify this date only if the item has Special Price" defaultValue="1900-01-01">
-      <questionPr top="2297" left="1" width="432" height="79" position="absolute"/>
+      <questionPr top="2395" left="1" width="432" height="79" position="absolute"/>
     </question>
     <question binding="26" text="Special Price To Date:" type="date" helpText="Only specify this date(Higher than Price From date) if only the item has Special price" defaultValue="2999-12-30">
-      <questionPr top="2381" left="1" width="432" height="93" position="absolute"/>
+      <questionPr top="2479" left="1" width="432" height="93" position="absolute"/>
     </question>
   </questions>
 </survey>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z4" totalsRowShown="0">
-  <autoFilter ref="A1:Z3"/>
-  <tableColumns count="26">
-    <tableColumn id="1" name="Category"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA4" totalsRowShown="0">
+  <autoFilter ref="A1:AA4"/>
+  <tableColumns count="27">
+    <tableColumn id="1" name="Category Name:"/>
     <tableColumn id="2" name="SKU Code:"/>
     <tableColumn id="3" name="Name:"/>
     <tableColumn id="4" name="Short Description:"/>
@@ -319,6 +401,7 @@
     <tableColumn id="9" name="Quantity:"/>
     <tableColumn id="10" name="Item Condition:"/>
     <tableColumn id="11" name="Seller Information:"/>
+    <tableColumn id="29" name="Currency Code:" dataDxfId="3"/>
     <tableColumn id="12" name="Price:"/>
     <tableColumn id="13" name="Cost Price:"/>
     <tableColumn id="14" name="List Price:"/>
@@ -602,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -619,7 +702,7 @@
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" customWidth="1"/>
@@ -633,9 +716,10 @@
     <col min="23" max="23" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="20.7109375" customWidth="1"/>
+    <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="45">
+    <row r="1" spans="1:27" ht="45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,28 +798,31 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="60">
+    <row r="2" spans="1:27" ht="75">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -744,13 +831,13 @@
         <v>1000</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="M2" s="1">
         <v>1</v>
@@ -761,17 +848,17 @@
       <c r="O2" s="1">
         <v>1</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>33</v>
+      <c r="P2" s="1">
+        <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
@@ -779,37 +866,40 @@
       <c r="U2" s="1">
         <v>0</v>
       </c>
-      <c r="V2" s="1" t="b">
+      <c r="V2" s="1">
         <v>0</v>
       </c>
       <c r="W2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X2" s="1"/>
+      <c r="X2" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="60">
+    <row r="3" spans="1:27" ht="75">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -818,34 +908,34 @@
         <v>1000</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="1">
+        <v>38</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1">
         <v>100</v>
-      </c>
-      <c r="M3" s="1">
-        <v>99</v>
       </c>
       <c r="N3" s="1">
         <v>99</v>
       </c>
       <c r="O3" s="1">
+        <v>99</v>
+      </c>
+      <c r="P3" s="1">
         <v>98</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="1">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="T3" s="1">
         <v>10</v>
@@ -853,90 +943,100 @@
       <c r="U3" s="1">
         <v>10</v>
       </c>
-      <c r="V3" s="1" t="b">
-        <v>1</v>
+      <c r="V3" s="1">
+        <v>10</v>
       </c>
       <c r="W3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="X3" s="1"/>
+      <c r="X3" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="60">
+    <row r="4" spans="1:27" ht="75">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H4" s="1">
+        <v>500</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1001</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="1">
+        <v>100</v>
+      </c>
+      <c r="N4" s="1">
+        <v>90</v>
+      </c>
+      <c r="O4" s="1">
+        <v>95</v>
+      </c>
+      <c r="P4" s="1">
+        <v>94</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" s="1">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1">
+        <v>10</v>
+      </c>
+      <c r="V4" s="1">
+        <v>10</v>
+      </c>
+      <c r="W4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="X4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-      <c r="V4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="X4" s="1">
-        <v>23</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>41840</v>
+      <c r="Y4" s="1">
+        <v>93</v>
       </c>
       <c r="Z4" s="3">
-        <v>41941</v>
+        <v>41842</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>42207</v>
       </c>
     </row>
   </sheetData>
@@ -949,12 +1049,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>225</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
change finally import tested
</commit_message>
<xml_diff>
--- a/SageFrame/Modules/AspxCommerce/AspxImportManager/Uploads/eCommerce Data Entry online.xlsx
+++ b/SageFrame/Modules/AspxCommerce/AspxImportManager/Uploads/eCommerce Data Entry online.xlsx
@@ -3,20 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Repo\AspxCommerce\BuyNSellNepal\SageFrame\Modules\AspxCommerce\AspxImportManager\Uploads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>Category Name:</t>
   </si>
@@ -156,9 +161,6 @@
     <t>fdsfa.jpg</t>
   </si>
   <si>
-    <t>fdsafd.jpg</t>
-  </si>
-  <si>
     <t>Not Specified</t>
   </si>
   <si>
@@ -211,13 +213,28 @@
   </si>
   <si>
     <t>60ml</t>
+  </si>
+  <si>
+    <t>test2.jpg</t>
+  </si>
+  <si>
+    <t>test.jpg</t>
+  </si>
+  <si>
+    <t>test_thumb.jpg</t>
+  </si>
+  <si>
+    <t>test2_thumb.jpg</t>
+  </si>
+  <si>
+    <t>fdsafd_thumb.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,10 +444,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -687,9 +704,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -719,7 +738,7 @@
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="45">
+    <row r="1" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +821,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="75">
+    <row r="2" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -819,10 +838,10 @@
         <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -879,7 +898,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" ht="75">
+    <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -896,10 +915,10 @@
         <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -956,7 +975,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="75">
+    <row r="4" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -976,7 +995,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="H4" s="1">
         <v>500</v>
@@ -985,10 +1004,10 @@
         <v>1001</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>34</v>
@@ -1006,13 +1025,13 @@
         <v>94</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T4" s="1">
         <v>10</v>
@@ -1051,9 +1070,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1063,33 +1082,33 @@
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1103,19 +1122,19 @@
         <v>100</v>
       </c>
       <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
         <v>58</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1129,16 +1148,16 @@
         <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1152,16 +1171,16 @@
         <v>150</v>
       </c>
       <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
         <v>62</v>
-      </c>
-      <c r="F4" t="s">
-        <v>63</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1175,10 +1194,10 @@
         <v>225</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -1195,7 +1214,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the name and price
</commit_message>
<xml_diff>
--- a/SageFrame/Modules/AspxCommerce/AspxImportManager/Uploads/eCommerce Data Entry online.xlsx
+++ b/SageFrame/Modules/AspxCommerce/AspxImportManager/Uploads/eCommerce Data Entry online.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Repo\AspxCommerce\BuyNSellNepal\SageFrame\Modules\AspxCommerce\AspxImportManager\Uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Repo\AspxCommerce\!@AspxCommerce3.0\SageFrame\Modules\AspxCommerce\AspxImportManager\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Category Name:</t>
   </si>
@@ -104,27 +104,12 @@
     <t>Special Price To Date:</t>
   </si>
   <si>
-    <t>Electronics/Cell Phones/Cell Phones &amp; Smartphones</t>
-  </si>
-  <si>
     <t>SKU01</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>teset</t>
-  </si>
-  <si>
-    <t>tse</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
-    <t>estestt etgdsg</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -134,39 +119,12 @@
     <t>SKU02</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
     <t>Used</t>
   </si>
   <si>
-    <t>sfdsf</t>
-  </si>
-  <si>
-    <t>dsfdsf</t>
-  </si>
-  <si>
-    <t>fdsf</t>
-  </si>
-  <si>
-    <t>fdsaf</t>
-  </si>
-  <si>
-    <t>dasfd</t>
-  </si>
-  <si>
-    <t>fdsfa.jpg</t>
-  </si>
-  <si>
     <t>Not Specified</t>
   </si>
   <si>
-    <t>fdsafdsafdsaf</t>
-  </si>
-  <si>
     <t>ecommerce, online shopping, nepalsss</t>
   </si>
   <si>
@@ -200,9 +158,6 @@
     <t>red</t>
   </si>
   <si>
-    <t>a.jpg,b.jpg</t>
-  </si>
-  <si>
     <t>green</t>
   </si>
   <si>
@@ -215,22 +170,49 @@
     <t>60ml</t>
   </si>
   <si>
-    <t>test2.jpg</t>
-  </si>
-  <si>
-    <t>test.jpg</t>
-  </si>
-  <si>
-    <t>test_thumb.jpg</t>
-  </si>
-  <si>
-    <t>test2_thumb.jpg</t>
-  </si>
-  <si>
-    <t>fdsafd_thumb.jpg</t>
-  </si>
-  <si>
     <t>NPR</t>
+  </si>
+  <si>
+    <t>SKU03</t>
+  </si>
+  <si>
+    <t>ImportTest</t>
+  </si>
+  <si>
+    <t>ImportTest.jpg</t>
+  </si>
+  <si>
+    <t>ImportTest_thumb.jpg</t>
+  </si>
+  <si>
+    <t>ImportTest1.png</t>
+  </si>
+  <si>
+    <t>ImportTest1_thumb.png</t>
+  </si>
+  <si>
+    <t>ImportTest1</t>
+  </si>
+  <si>
+    <t>ImportTest2</t>
+  </si>
+  <si>
+    <t>ImportTest2.jpg</t>
+  </si>
+  <si>
+    <t>ImportTest2_thumb.jpg</t>
+  </si>
+  <si>
+    <t>Category1</t>
+  </si>
+  <si>
+    <t>Category1/SubCategory/ChildCategory</t>
+  </si>
+  <si>
+    <t>Category2</t>
+  </si>
+  <si>
+    <t>Seller detail location and contact and google map description here</t>
   </si>
 </sst>
 </file>
@@ -707,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,25 +808,25 @@
     </row>
     <row r="2" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -853,32 +835,32 @@
         <v>1000</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="M2" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="O2" s="1">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
@@ -901,61 +883,61 @@
     </row>
     <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I3" s="2">
         <v>1000</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1">
+        <v>150</v>
+      </c>
+      <c r="N3" s="1">
         <v>100</v>
       </c>
-      <c r="N3" s="1">
-        <v>99</v>
-      </c>
       <c r="O3" s="1">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="P3" s="1">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T3" s="1">
         <v>10</v>
@@ -978,40 +960,40 @@
     </row>
     <row r="4" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H4" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2">
         <v>1001</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="M4" s="1">
         <v>100</v>
@@ -1026,19 +1008,19 @@
         <v>94</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="T4" s="1">
         <v>10</v>
       </c>
       <c r="U4" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="V4" s="1">
         <v>10</v>
@@ -1050,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="Y4" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z4" s="3">
         <v>41842</v>
@@ -1072,7 +1054,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,59 +1069,56 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>80</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G2">
         <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1148,13 +1127,13 @@
         <v>20</v>
       </c>
       <c r="D3">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1162,7 +1141,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1171,13 +1150,13 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1185,7 +1164,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1197,10 +1176,10 @@
         <v>225</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G5">
         <v>2</v>

</xml_diff>